<commit_message>
Jang Junho and 장준호
</commit_message>
<xml_diff>
--- a/data/2020-02-11/Senior Cubers Worldwide - Weekly Competition - 2020-02-11.xlsx
+++ b/data/2020-02-11/Senior Cubers Worldwide - Weekly Competition - 2020-02-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB72BBA-8B27-465E-95D3-94AF34DA8152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E298A-BA29-4A14-B7D7-920C2DBB6D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>https://www.facebook.com/events/616423959107229/permalink/617588112324147/</t>
   </si>
   <si>
-    <t>Jang Junho</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/events/616423959107229/permalink/618758058873819/</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>Jamie Brady (Deansie)</t>
+  </si>
+  <si>
+    <t>Jang Junho (장준호)</t>
   </si>
 </sst>
 </file>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A1:K1032"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1046,7 +1046,7 @@
         <v>12.93</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="15">
         <v>15.03</v>
@@ -1185,7 +1185,7 @@
         <v>18.350000000000001</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F9" s="19">
         <v>15.52</v>
@@ -1254,7 +1254,7 @@
         <v>18.79333333333334</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" s="19">
         <v>16.2</v>
@@ -1322,7 +1322,7 @@
         <v>19.48</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="19">
         <v>17.28</v>
@@ -1425,7 +1425,7 @@
         <v>23.45</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="19">
         <v>21.85</v>
@@ -1493,7 +1493,7 @@
         <v>23.99</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="19">
         <v>19.62</v>
@@ -1519,7 +1519,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>30</v>
@@ -1588,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>30</v>
@@ -1621,7 +1621,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>75</v>
@@ -1631,7 +1631,7 @@
         <v>28.956666666666663</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22" s="19">
         <v>28.44</v>
@@ -1666,7 +1666,7 @@
         <v>29.37</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="19">
         <v>28.16</v>
@@ -1692,7 +1692,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>20</v>
@@ -1717,7 +1717,7 @@
         <v>30.87</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="12.75">
@@ -1750,7 +1750,7 @@
         <v>37</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="12.75">
@@ -1783,7 +1783,7 @@
         <v>39.46</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75">
@@ -1791,7 +1791,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>75</v>
@@ -1800,7 +1800,7 @@
         <v>35.21</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F27" s="19">
         <v>34.54</v>
@@ -1835,7 +1835,7 @@
         <v>38.799999999999997</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28" s="19">
         <v>47.44</v>
@@ -1853,7 +1853,7 @@
         <v>35.6</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="12.75">
@@ -1861,7 +1861,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>75</v>
@@ -1870,7 +1870,7 @@
         <v>40.880000000000003</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F29" s="19">
         <v>40.409999999999997</v>
@@ -1888,7 +1888,7 @@
         <v>31.38</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75">
@@ -1921,7 +1921,7 @@
         <v>32</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="12.75">
@@ -1935,11 +1935,11 @@
         <v>20</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G31" s="43">
         <v>59.4</v>
@@ -1948,13 +1948,13 @@
         <v>32</v>
       </c>
       <c r="I31" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J31" s="43">
         <v>58.55</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="12.75">
@@ -8564,7 +8564,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>75</v>
@@ -21483,7 +21483,7 @@
   </sheetPr>
   <dimension ref="A1:F1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -21501,7 +21501,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -21527,13 +21527,13 @@
         <v>6</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
@@ -21553,7 +21553,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75">
@@ -21561,7 +21561,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>20</v>
@@ -21573,7 +21573,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75">
@@ -21581,7 +21581,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>75</v>
@@ -21593,7 +21593,7 @@
         <v>43</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75">
@@ -21611,7 +21611,7 @@
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75">
@@ -21619,7 +21619,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>30</v>
@@ -21629,7 +21629,7 @@
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75">
@@ -21647,7 +21647,7 @@
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75">
@@ -21665,7 +21665,7 @@
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75">
@@ -21673,7 +21673,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>75</v>
@@ -21683,7 +21683,7 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75">

</xml_diff>